<commit_message>
update get only trends
Antes era necesario hacer todo el proceso de forecasting para obtener tambien las tendencias, con esta nueva opcion es posible solo obtener las tendencias de manera masiva
</commit_message>
<xml_diff>
--- a/Streamlit_test/Examples/FRTS.xlsx
+++ b/Streamlit_test/Examples/FRTS.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabri\Documents\python codes\Streamlit_test\Examples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabri\Documents\GitHub\Proyeccionconsumo_stl\Streamlit_test\Examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B7ABFE8-C3EC-47D1-842F-35D47362F5DE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D5233C2-4DD2-4753-8130-C9EFBC1290C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C796BCA3-2FA4-4664-94CB-1CAFA793BC87}"/>
   </bookViews>
@@ -28,15 +28,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>FRTS</t>
   </si>
   <si>
-    <t>frt38355</t>
-  </si>
-  <si>
-    <t>frt38868</t>
+    <t>TOTAL</t>
   </si>
 </sst>
 </file>
@@ -394,10 +391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8873190-3545-473C-830E-FD76C1CEE33F}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3:A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -412,11 +409,6 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-    </row>
   </sheetData>
   <autoFilter ref="A1:A646" xr:uid="{BDE87B57-CA50-471E-9D28-0CEA53816AD9}"/>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>